<commit_message>
Change missing values in Q1 column from Undecided to None
</commit_message>
<xml_diff>
--- a/generated_report.xlsx
+++ b/generated_report.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jeebe\Test-Code\python-stuff\takehomes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046340BB-B5A1-46A9-91F2-668D94EA7672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-23148" yWindow="4368" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -64,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +134,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +220,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +272,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +465,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -465,7 +517,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -488,7 +540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -511,7 +563,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -534,7 +586,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -557,7 +609,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -580,7 +632,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -603,30 +655,30 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>1130</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>867</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>821</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>856</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>678</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>4352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>